<commit_message>
- Add Query strongly typed mapping - Add QueryFirstOrDefault、QuerySingle、QuerySingleOrDefault
</commit_message>
<xml_diff>
--- a/samples/xlsx/TestTypeMapping.xlsx
+++ b/samples/xlsx/TestTypeMapping.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\git\MiniExcel\samples\xlsx\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BEE6092B-66A5-486F-9479-3A7DBAC74B95}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7725CD23-B626-49D6-88CC-412E88C9EB67}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-21720" yWindow="-120" windowWidth="21840" windowHeight="13290" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="507" uniqueCount="401">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="508" uniqueCount="402">
   <si>
     <t>ID</t>
   </si>
@@ -1223,17 +1223,33 @@
   </si>
   <si>
     <t>tellus.Phasellus.elit@Etiamlaoreetlibero.edu</t>
+  </si>
+  <si>
+    <t>IgnoredProperty</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -1253,13 +1269,17 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -1562,2339 +1582,2355 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G101"/>
+  <dimension ref="A1:H101"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G1" sqref="G1"/>
+      <selection activeCell="J2" sqref="J2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="28.21875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="8.33203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="8.109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="2.88671875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="4" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="17.109375" customWidth="1"/>
+    <col min="7" max="7" width="6.21875" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A1" t="s">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
+      <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" t="s">
+      <c r="E1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" t="s">
+      <c r="F1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="G1" t="s">
+      <c r="G1" s="1" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
+      <c r="H1" s="1" t="s">
+        <v>401</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A2" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B2" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="C2" t="s">
+      <c r="C2" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="D2">
+      <c r="D2" s="1">
         <v>36</v>
       </c>
-      <c r="E2" t="s">
-        <v>10</v>
-      </c>
-      <c r="F2" t="s">
+      <c r="E2" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="F2" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="G2">
+      <c r="G2" s="1">
         <v>5019.12</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A3" t="s">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A3" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B3" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="C3" t="s">
+      <c r="C3" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="D3">
+      <c r="D3" s="1">
         <v>44</v>
       </c>
-      <c r="E3" t="s">
-        <v>15</v>
-      </c>
-      <c r="F3" t="s">
+      <c r="E3" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="F3" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="G3">
+      <c r="G3" s="1">
         <v>7028.46</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A4" t="s">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A4" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="B4" t="s">
+      <c r="B4" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="C4" t="s">
+      <c r="C4" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="D4">
+      <c r="D4" s="1">
         <v>33</v>
       </c>
-      <c r="E4" t="s">
-        <v>15</v>
-      </c>
-      <c r="F4" t="s">
+      <c r="E4" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="F4" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="G4">
+      <c r="G4" s="1">
         <v>3835.7</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A5" t="s">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A5" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="B5" t="s">
+      <c r="B5" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="C5" t="s">
+      <c r="C5" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="D5">
+      <c r="D5" s="1">
         <v>32</v>
       </c>
-      <c r="E5" t="s">
-        <v>10</v>
-      </c>
-      <c r="F5" t="s">
+      <c r="E5" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="F5" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="G5">
+      <c r="G5" s="1">
         <v>9351.7099999999991</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A6" t="s">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A6" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="B6" t="s">
+      <c r="B6" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="C6" t="s">
+      <c r="C6" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="D6">
+      <c r="D6" s="1">
         <v>18</v>
       </c>
-      <c r="E6" t="s">
-        <v>15</v>
-      </c>
-      <c r="F6" t="s">
+      <c r="E6" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="F6" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="G6">
+      <c r="G6" s="1">
         <v>8209.76</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A7" t="s">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A7" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="B7" t="s">
+      <c r="B7" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="C7" t="s">
+      <c r="C7" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="D7">
+      <c r="D7" s="1">
         <v>60</v>
       </c>
-      <c r="E7" t="s">
-        <v>10</v>
-      </c>
-      <c r="F7" t="s">
+      <c r="E7" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="F7" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="G7">
+      <c r="G7" s="1">
         <v>4288.18</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A8" t="s">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A8" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="B8" t="s">
+      <c r="B8" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="C8" t="s">
+      <c r="C8" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="D8">
+      <c r="D8" s="1">
         <v>30</v>
       </c>
-      <c r="E8" t="s">
-        <v>10</v>
-      </c>
-      <c r="F8" t="s">
+      <c r="E8" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="F8" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="G8">
+      <c r="G8" s="1">
         <v>3248.12</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A9" t="s">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A9" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="B9" t="s">
+      <c r="B9" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="C9" t="s">
+      <c r="C9" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="D9">
+      <c r="D9" s="1">
         <v>52</v>
       </c>
-      <c r="E9" t="s">
-        <v>15</v>
-      </c>
-      <c r="F9" t="s">
+      <c r="E9" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="F9" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="G9">
+      <c r="G9" s="1">
         <v>2586.66</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A10" t="s">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A10" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="B10" t="s">
+      <c r="B10" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="C10" t="s">
+      <c r="C10" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="D10">
+      <c r="D10" s="1">
         <v>34</v>
       </c>
-      <c r="E10" t="s">
-        <v>15</v>
-      </c>
-      <c r="F10" t="s">
+      <c r="E10" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="F10" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="G10">
+      <c r="G10" s="1">
         <v>5970.74</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A11" t="s">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A11" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="B11" t="s">
+      <c r="B11" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="C11" t="s">
+      <c r="C11" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="D11">
+      <c r="D11" s="1">
         <v>43</v>
       </c>
-      <c r="E11" t="s">
-        <v>10</v>
-      </c>
-      <c r="F11" t="s">
+      <c r="E11" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="F11" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="G11">
+      <c r="G11" s="1">
         <v>1057.57</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A12" t="s">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A12" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="B12" t="s">
+      <c r="B12" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="C12" t="s">
+      <c r="C12" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="D12">
+      <c r="D12" s="1">
         <v>47</v>
       </c>
-      <c r="E12" t="s">
-        <v>10</v>
-      </c>
-      <c r="F12" t="s">
+      <c r="E12" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="F12" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="G12">
+      <c r="G12" s="1">
         <v>9307.98</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A13" t="s">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A13" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="B13" t="s">
+      <c r="B13" s="1" t="s">
         <v>54</v>
       </c>
-      <c r="C13" t="s">
+      <c r="C13" s="1" t="s">
         <v>55</v>
       </c>
-      <c r="D13">
+      <c r="D13" s="1">
         <v>44</v>
       </c>
-      <c r="E13" t="s">
-        <v>15</v>
-      </c>
-      <c r="F13" t="s">
+      <c r="E13" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="F13" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="G13">
+      <c r="G13" s="1">
         <v>6389.64</v>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A14" t="s">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A14" s="1" t="s">
         <v>57</v>
       </c>
-      <c r="B14" t="s">
+      <c r="B14" s="1" t="s">
         <v>58</v>
       </c>
-      <c r="C14" t="s">
+      <c r="C14" s="1" t="s">
         <v>59</v>
       </c>
-      <c r="D14">
+      <c r="D14" s="1">
         <v>52</v>
       </c>
-      <c r="E14" t="s">
-        <v>10</v>
-      </c>
-      <c r="F14" t="s">
+      <c r="E14" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="F14" s="1" t="s">
         <v>60</v>
       </c>
-      <c r="G14">
+      <c r="G14" s="1">
         <v>8804.6</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A15" t="s">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A15" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="B15" t="s">
+      <c r="B15" s="1" t="s">
         <v>62</v>
       </c>
-      <c r="C15" t="s">
+      <c r="C15" s="1" t="s">
         <v>63</v>
       </c>
-      <c r="D15">
+      <c r="D15" s="1">
         <v>54</v>
       </c>
-      <c r="E15" t="s">
-        <v>15</v>
-      </c>
-      <c r="F15" t="s">
+      <c r="E15" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="F15" s="1" t="s">
         <v>64</v>
       </c>
-      <c r="G15">
+      <c r="G15" s="1">
         <v>8527.6299999999992</v>
       </c>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A16" t="s">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A16" s="1" t="s">
         <v>65</v>
       </c>
-      <c r="B16" t="s">
+      <c r="B16" s="1" t="s">
         <v>66</v>
       </c>
-      <c r="C16" t="s">
+      <c r="C16" s="1" t="s">
         <v>67</v>
       </c>
-      <c r="D16">
+      <c r="D16" s="1">
         <v>51</v>
       </c>
-      <c r="E16" t="s">
-        <v>15</v>
-      </c>
-      <c r="F16" t="s">
+      <c r="E16" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="F16" s="1" t="s">
         <v>68</v>
       </c>
-      <c r="G16">
+      <c r="G16" s="1">
         <v>4616.82</v>
       </c>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A17" t="s">
+      <c r="A17" s="1" t="s">
         <v>69</v>
       </c>
-      <c r="B17" t="s">
+      <c r="B17" s="1" t="s">
         <v>70</v>
       </c>
-      <c r="C17" t="s">
+      <c r="C17" s="1" t="s">
         <v>71</v>
       </c>
-      <c r="D17">
+      <c r="D17" s="1">
         <v>20</v>
       </c>
-      <c r="E17" t="s">
-        <v>10</v>
-      </c>
-      <c r="F17" t="s">
+      <c r="E17" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="F17" s="1" t="s">
         <v>72</v>
       </c>
-      <c r="G17">
+      <c r="G17" s="1">
         <v>401.75</v>
       </c>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A18" t="s">
+      <c r="A18" s="1" t="s">
         <v>73</v>
       </c>
-      <c r="B18" t="s">
+      <c r="B18" s="1" t="s">
         <v>74</v>
       </c>
-      <c r="C18" t="s">
+      <c r="C18" s="1" t="s">
         <v>75</v>
       </c>
-      <c r="D18">
+      <c r="D18" s="1">
         <v>23</v>
       </c>
-      <c r="E18" t="s">
-        <v>15</v>
-      </c>
-      <c r="F18" t="s">
+      <c r="E18" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="F18" s="1" t="s">
         <v>76</v>
       </c>
-      <c r="G18">
+      <c r="G18" s="1">
         <v>5624.33</v>
       </c>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A19" t="s">
+      <c r="A19" s="1" t="s">
         <v>77</v>
       </c>
-      <c r="B19" t="s">
+      <c r="B19" s="1" t="s">
         <v>78</v>
       </c>
-      <c r="C19" t="s">
+      <c r="C19" s="1" t="s">
         <v>79</v>
       </c>
-      <c r="D19">
+      <c r="D19" s="1">
         <v>20</v>
       </c>
-      <c r="E19" t="s">
-        <v>15</v>
-      </c>
-      <c r="F19" t="s">
+      <c r="E19" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="F19" s="1" t="s">
         <v>80</v>
       </c>
-      <c r="G19">
+      <c r="G19" s="1">
         <v>123.2</v>
       </c>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A20" t="s">
+      <c r="A20" s="1" t="s">
         <v>81</v>
       </c>
-      <c r="B20" t="s">
+      <c r="B20" s="1" t="s">
         <v>82</v>
       </c>
-      <c r="C20" t="s">
+      <c r="C20" s="1" t="s">
         <v>83</v>
       </c>
-      <c r="D20">
+      <c r="D20" s="1">
         <v>38</v>
       </c>
-      <c r="E20" t="s">
-        <v>15</v>
-      </c>
-      <c r="F20" t="s">
+      <c r="E20" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="F20" s="1" t="s">
         <v>84</v>
       </c>
-      <c r="G20">
+      <c r="G20" s="1">
         <v>6161.41</v>
       </c>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A21" t="s">
+      <c r="A21" s="1" t="s">
         <v>85</v>
       </c>
-      <c r="B21" t="s">
+      <c r="B21" s="1" t="s">
         <v>86</v>
       </c>
-      <c r="C21" t="s">
+      <c r="C21" s="1" t="s">
         <v>87</v>
       </c>
-      <c r="D21">
+      <c r="D21" s="1">
         <v>26</v>
       </c>
-      <c r="E21" t="s">
-        <v>10</v>
-      </c>
-      <c r="F21" t="s">
+      <c r="E21" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="F21" s="1" t="s">
         <v>88</v>
       </c>
-      <c r="G21">
+      <c r="G21" s="1">
         <v>5616.12</v>
       </c>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A22" t="s">
+      <c r="A22" s="1" t="s">
         <v>89</v>
       </c>
-      <c r="B22" t="s">
+      <c r="B22" s="1" t="s">
         <v>90</v>
       </c>
-      <c r="C22" t="s">
+      <c r="C22" s="1" t="s">
         <v>91</v>
       </c>
-      <c r="D22">
+      <c r="D22" s="1">
         <v>54</v>
       </c>
-      <c r="E22" t="s">
-        <v>15</v>
-      </c>
-      <c r="F22" t="s">
+      <c r="E22" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="F22" s="1" t="s">
         <v>92</v>
       </c>
-      <c r="G22">
+      <c r="G22" s="1">
         <v>844.25</v>
       </c>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A23" t="s">
+      <c r="A23" s="1" t="s">
         <v>93</v>
       </c>
-      <c r="B23" t="s">
+      <c r="B23" s="1" t="s">
         <v>94</v>
       </c>
-      <c r="C23" t="s">
+      <c r="C23" s="1" t="s">
         <v>95</v>
       </c>
-      <c r="D23">
+      <c r="D23" s="1">
         <v>48</v>
       </c>
-      <c r="E23" t="s">
-        <v>15</v>
-      </c>
-      <c r="F23" t="s">
+      <c r="E23" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="F23" s="1" t="s">
         <v>96</v>
       </c>
-      <c r="G23">
+      <c r="G23" s="1">
         <v>1891.27</v>
       </c>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A24" t="s">
+      <c r="A24" s="1" t="s">
         <v>97</v>
       </c>
-      <c r="B24" t="s">
+      <c r="B24" s="1" t="s">
         <v>98</v>
       </c>
-      <c r="C24" t="s">
+      <c r="C24" s="1" t="s">
         <v>99</v>
       </c>
-      <c r="D24">
+      <c r="D24" s="1">
         <v>36</v>
       </c>
-      <c r="E24" t="s">
-        <v>10</v>
-      </c>
-      <c r="F24" t="s">
+      <c r="E24" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="F24" s="1" t="s">
         <v>100</v>
       </c>
-      <c r="G24">
+      <c r="G24" s="1">
         <v>642.92999999999995</v>
       </c>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A25" t="s">
+      <c r="A25" s="1" t="s">
         <v>101</v>
       </c>
-      <c r="B25" t="s">
+      <c r="B25" s="1" t="s">
         <v>102</v>
       </c>
-      <c r="C25" t="s">
+      <c r="C25" s="1" t="s">
         <v>103</v>
       </c>
-      <c r="D25">
+      <c r="D25" s="1">
         <v>39</v>
       </c>
-      <c r="E25" t="s">
-        <v>10</v>
-      </c>
-      <c r="F25" t="s">
+      <c r="E25" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="F25" s="1" t="s">
         <v>104</v>
       </c>
-      <c r="G25">
+      <c r="G25" s="1">
         <v>2320.4899999999998</v>
       </c>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A26" t="s">
+      <c r="A26" s="1" t="s">
         <v>105</v>
       </c>
-      <c r="B26" t="s">
+      <c r="B26" s="1" t="s">
         <v>106</v>
       </c>
-      <c r="C26" t="s">
+      <c r="C26" s="1" t="s">
         <v>107</v>
       </c>
-      <c r="D26">
+      <c r="D26" s="1">
         <v>54</v>
       </c>
-      <c r="E26" t="s">
-        <v>10</v>
-      </c>
-      <c r="F26" t="s">
+      <c r="E26" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="F26" s="1" t="s">
         <v>108</v>
       </c>
-      <c r="G26">
+      <c r="G26" s="1">
         <v>6947.08</v>
       </c>
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A27" t="s">
+      <c r="A27" s="1" t="s">
         <v>109</v>
       </c>
-      <c r="B27" t="s">
+      <c r="B27" s="1" t="s">
         <v>110</v>
       </c>
-      <c r="C27" t="s">
+      <c r="C27" s="1" t="s">
         <v>111</v>
       </c>
-      <c r="D27">
+      <c r="D27" s="1">
         <v>39</v>
       </c>
-      <c r="E27" t="s">
-        <v>15</v>
-      </c>
-      <c r="F27" t="s">
+      <c r="E27" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="F27" s="1" t="s">
         <v>112</v>
       </c>
-      <c r="G27">
+      <c r="G27" s="1">
         <v>9052.67</v>
       </c>
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A28" t="s">
+      <c r="A28" s="1" t="s">
         <v>113</v>
       </c>
-      <c r="B28" t="s">
+      <c r="B28" s="1" t="s">
         <v>114</v>
       </c>
-      <c r="C28" t="s">
+      <c r="C28" s="1" t="s">
         <v>115</v>
       </c>
-      <c r="D28">
+      <c r="D28" s="1">
         <v>31</v>
       </c>
-      <c r="E28" t="s">
-        <v>15</v>
-      </c>
-      <c r="F28" t="s">
+      <c r="E28" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="F28" s="1" t="s">
         <v>116</v>
       </c>
-      <c r="G28">
+      <c r="G28" s="1">
         <v>9364.1200000000008</v>
       </c>
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A29" t="s">
+      <c r="A29" s="1" t="s">
         <v>117</v>
       </c>
-      <c r="B29" t="s">
+      <c r="B29" s="1" t="s">
         <v>118</v>
       </c>
-      <c r="C29" t="s">
+      <c r="C29" s="1" t="s">
         <v>119</v>
       </c>
-      <c r="D29">
+      <c r="D29" s="1">
         <v>33</v>
       </c>
-      <c r="E29" t="s">
-        <v>10</v>
-      </c>
-      <c r="F29" t="s">
+      <c r="E29" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="F29" s="1" t="s">
         <v>120</v>
       </c>
-      <c r="G29">
+      <c r="G29" s="1">
         <v>5542.36</v>
       </c>
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A30" t="s">
+      <c r="A30" s="1" t="s">
         <v>121</v>
       </c>
-      <c r="B30" t="s">
+      <c r="B30" s="1" t="s">
         <v>122</v>
       </c>
-      <c r="C30" t="s">
+      <c r="C30" s="1" t="s">
         <v>123</v>
       </c>
-      <c r="D30">
+      <c r="D30" s="1">
         <v>43</v>
       </c>
-      <c r="E30" t="s">
-        <v>15</v>
-      </c>
-      <c r="F30" t="s">
+      <c r="E30" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="F30" s="1" t="s">
         <v>124</v>
       </c>
-      <c r="G30">
+      <c r="G30" s="1">
         <v>2846.99</v>
       </c>
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A31" t="s">
+      <c r="A31" s="1" t="s">
         <v>125</v>
       </c>
-      <c r="B31" t="s">
+      <c r="B31" s="1" t="s">
         <v>126</v>
       </c>
-      <c r="C31" t="s">
+      <c r="C31" s="1" t="s">
         <v>79</v>
       </c>
-      <c r="D31">
+      <c r="D31" s="1">
         <v>40</v>
       </c>
-      <c r="E31" t="s">
-        <v>15</v>
-      </c>
-      <c r="F31" t="s">
+      <c r="E31" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="F31" s="1" t="s">
         <v>127</v>
       </c>
-      <c r="G31">
+      <c r="G31" s="1">
         <v>4930.8599999999997</v>
       </c>
     </row>
     <row r="32" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A32" t="s">
+      <c r="A32" s="1" t="s">
         <v>128</v>
       </c>
-      <c r="B32" t="s">
+      <c r="B32" s="1" t="s">
         <v>129</v>
       </c>
-      <c r="C32" t="s">
+      <c r="C32" s="1" t="s">
         <v>130</v>
       </c>
-      <c r="D32">
+      <c r="D32" s="1">
         <v>27</v>
       </c>
-      <c r="E32" t="s">
-        <v>10</v>
-      </c>
-      <c r="F32" t="s">
+      <c r="E32" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="F32" s="1" t="s">
         <v>131</v>
       </c>
-      <c r="G32">
+      <c r="G32" s="1">
         <v>2008.3</v>
       </c>
     </row>
     <row r="33" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A33" t="s">
+      <c r="A33" s="1" t="s">
         <v>132</v>
       </c>
-      <c r="B33" t="s">
+      <c r="B33" s="1" t="s">
         <v>133</v>
       </c>
-      <c r="C33" t="s">
+      <c r="C33" s="1" t="s">
         <v>134</v>
       </c>
-      <c r="D33">
+      <c r="D33" s="1">
         <v>28</v>
       </c>
-      <c r="E33" t="s">
-        <v>10</v>
-      </c>
-      <c r="F33" t="s">
+      <c r="E33" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="F33" s="1" t="s">
         <v>135</v>
       </c>
-      <c r="G33">
+      <c r="G33" s="1">
         <v>1527.49</v>
       </c>
     </row>
     <row r="34" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A34" t="s">
+      <c r="A34" s="1" t="s">
         <v>136</v>
       </c>
-      <c r="B34" t="s">
+      <c r="B34" s="1" t="s">
         <v>137</v>
       </c>
-      <c r="C34" t="s">
+      <c r="C34" s="1" t="s">
         <v>138</v>
       </c>
-      <c r="D34">
+      <c r="D34" s="1">
         <v>21</v>
       </c>
-      <c r="E34" t="s">
-        <v>15</v>
-      </c>
-      <c r="F34" t="s">
+      <c r="E34" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="F34" s="1" t="s">
         <v>139</v>
       </c>
-      <c r="G34">
+      <c r="G34" s="1">
         <v>1850.07</v>
       </c>
     </row>
     <row r="35" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A35" t="s">
+      <c r="A35" s="1" t="s">
         <v>140</v>
       </c>
-      <c r="B35" t="s">
+      <c r="B35" s="1" t="s">
         <v>141</v>
       </c>
-      <c r="C35" t="s">
+      <c r="C35" s="1" t="s">
         <v>142</v>
       </c>
-      <c r="D35">
+      <c r="D35" s="1">
         <v>50</v>
       </c>
-      <c r="E35" t="s">
-        <v>10</v>
-      </c>
-      <c r="F35" t="s">
+      <c r="E35" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="F35" s="1" t="s">
         <v>143</v>
       </c>
-      <c r="G35">
+      <c r="G35" s="1">
         <v>6070.33</v>
       </c>
     </row>
     <row r="36" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A36" t="s">
+      <c r="A36" s="1" t="s">
         <v>144</v>
       </c>
-      <c r="B36" t="s">
+      <c r="B36" s="1" t="s">
         <v>145</v>
       </c>
-      <c r="C36" t="s">
+      <c r="C36" s="1" t="s">
         <v>146</v>
       </c>
-      <c r="D36">
+      <c r="D36" s="1">
         <v>45</v>
       </c>
-      <c r="E36" t="s">
-        <v>10</v>
-      </c>
-      <c r="F36" t="s">
+      <c r="E36" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="F36" s="1" t="s">
         <v>147</v>
       </c>
-      <c r="G36">
+      <c r="G36" s="1">
         <v>1244.6500000000001</v>
       </c>
     </row>
     <row r="37" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A37" t="s">
+      <c r="A37" s="1" t="s">
         <v>148</v>
       </c>
-      <c r="B37" t="s">
+      <c r="B37" s="1" t="s">
         <v>149</v>
       </c>
-      <c r="C37" t="s">
+      <c r="C37" s="1" t="s">
         <v>150</v>
       </c>
-      <c r="D37">
+      <c r="D37" s="1">
         <v>43</v>
       </c>
-      <c r="E37" t="s">
-        <v>10</v>
-      </c>
-      <c r="F37" t="s">
+      <c r="E37" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="F37" s="1" t="s">
         <v>151</v>
       </c>
-      <c r="G37">
+      <c r="G37" s="1">
         <v>9777.42</v>
       </c>
     </row>
     <row r="38" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A38" t="s">
+      <c r="A38" s="1" t="s">
         <v>152</v>
       </c>
-      <c r="B38" t="s">
+      <c r="B38" s="1" t="s">
         <v>153</v>
       </c>
-      <c r="C38" t="s">
+      <c r="C38" s="1" t="s">
         <v>154</v>
       </c>
-      <c r="D38">
+      <c r="D38" s="1">
         <v>59</v>
       </c>
-      <c r="E38" t="s">
-        <v>15</v>
-      </c>
-      <c r="F38" t="s">
+      <c r="E38" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="F38" s="1" t="s">
         <v>155</v>
       </c>
-      <c r="G38">
+      <c r="G38" s="1">
         <v>4922.2700000000004</v>
       </c>
     </row>
     <row r="39" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A39" t="s">
+      <c r="A39" s="1" t="s">
         <v>156</v>
       </c>
-      <c r="B39" t="s">
+      <c r="B39" s="1" t="s">
         <v>157</v>
       </c>
-      <c r="C39" t="s">
+      <c r="C39" s="1" t="s">
         <v>158</v>
       </c>
-      <c r="D39">
+      <c r="D39" s="1">
         <v>38</v>
       </c>
-      <c r="E39" t="s">
-        <v>10</v>
-      </c>
-      <c r="F39" t="s">
+      <c r="E39" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="F39" s="1" t="s">
         <v>159</v>
       </c>
-      <c r="G39">
+      <c r="G39" s="1">
         <v>7241.36</v>
       </c>
     </row>
     <row r="40" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A40" t="s">
+      <c r="A40" s="1" t="s">
         <v>160</v>
       </c>
-      <c r="B40" t="s">
+      <c r="B40" s="1" t="s">
         <v>161</v>
       </c>
-      <c r="C40" t="s">
+      <c r="C40" s="1" t="s">
         <v>162</v>
       </c>
-      <c r="D40">
+      <c r="D40" s="1">
         <v>36</v>
       </c>
-      <c r="E40" t="s">
-        <v>10</v>
-      </c>
-      <c r="F40" t="s">
+      <c r="E40" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="F40" s="1" t="s">
         <v>163</v>
       </c>
-      <c r="G40">
+      <c r="G40" s="1">
         <v>3138.38</v>
       </c>
     </row>
     <row r="41" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A41" t="s">
+      <c r="A41" s="1" t="s">
         <v>164</v>
       </c>
-      <c r="B41" t="s">
+      <c r="B41" s="1" t="s">
         <v>165</v>
       </c>
-      <c r="C41" t="s">
+      <c r="C41" s="1" t="s">
         <v>166</v>
       </c>
-      <c r="D41">
+      <c r="D41" s="1">
         <v>56</v>
       </c>
-      <c r="E41" t="s">
-        <v>10</v>
-      </c>
-      <c r="F41" t="s">
+      <c r="E41" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="F41" s="1" t="s">
         <v>167</v>
       </c>
-      <c r="G41">
+      <c r="G41" s="1">
         <v>4646.3500000000004</v>
       </c>
     </row>
     <row r="42" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A42" t="s">
+      <c r="A42" s="1" t="s">
         <v>168</v>
       </c>
-      <c r="B42" t="s">
+      <c r="B42" s="1" t="s">
         <v>169</v>
       </c>
-      <c r="C42" t="s">
+      <c r="C42" s="1" t="s">
         <v>170</v>
       </c>
-      <c r="D42">
+      <c r="D42" s="1">
         <v>58</v>
       </c>
-      <c r="E42" t="s">
-        <v>15</v>
-      </c>
-      <c r="F42" t="s">
+      <c r="E42" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="F42" s="1" t="s">
         <v>171</v>
       </c>
-      <c r="G42">
+      <c r="G42" s="1">
         <v>2425.42</v>
       </c>
     </row>
     <row r="43" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A43" t="s">
+      <c r="A43" s="1" t="s">
         <v>172</v>
       </c>
-      <c r="B43" t="s">
+      <c r="B43" s="1" t="s">
         <v>173</v>
       </c>
-      <c r="C43" t="s">
+      <c r="C43" s="1" t="s">
         <v>174</v>
       </c>
-      <c r="D43">
+      <c r="D43" s="1">
         <v>21</v>
       </c>
-      <c r="E43" t="s">
-        <v>10</v>
-      </c>
-      <c r="F43" t="s">
+      <c r="E43" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="F43" s="1" t="s">
         <v>175</v>
       </c>
-      <c r="G43">
+      <c r="G43" s="1">
         <v>9757.07</v>
       </c>
     </row>
     <row r="44" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A44" t="s">
+      <c r="A44" s="1" t="s">
         <v>176</v>
       </c>
-      <c r="B44" t="s">
+      <c r="B44" s="1" t="s">
         <v>177</v>
       </c>
-      <c r="C44" t="s">
+      <c r="C44" s="1" t="s">
         <v>178</v>
       </c>
-      <c r="D44">
+      <c r="D44" s="1">
         <v>50</v>
       </c>
-      <c r="E44" t="s">
-        <v>15</v>
-      </c>
-      <c r="F44" t="s">
+      <c r="E44" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="F44" s="1" t="s">
         <v>179</v>
       </c>
-      <c r="G44">
+      <c r="G44" s="1">
         <v>1691.34</v>
       </c>
     </row>
     <row r="45" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A45" t="s">
+      <c r="A45" s="1" t="s">
         <v>180</v>
       </c>
-      <c r="B45" t="s">
+      <c r="B45" s="1" t="s">
         <v>181</v>
       </c>
-      <c r="C45" t="s">
+      <c r="C45" s="1" t="s">
         <v>182</v>
       </c>
-      <c r="D45">
+      <c r="D45" s="1">
         <v>43</v>
       </c>
-      <c r="E45" t="s">
-        <v>10</v>
-      </c>
-      <c r="F45" t="s">
+      <c r="E45" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="F45" s="1" t="s">
         <v>183</v>
       </c>
-      <c r="G45">
+      <c r="G45" s="1">
         <v>584.89</v>
       </c>
     </row>
     <row r="46" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A46" t="s">
+      <c r="A46" s="1" t="s">
         <v>184</v>
       </c>
-      <c r="B46" t="s">
+      <c r="B46" s="1" t="s">
         <v>185</v>
       </c>
-      <c r="C46" t="s">
+      <c r="C46" s="1" t="s">
         <v>186</v>
       </c>
-      <c r="D46">
+      <c r="D46" s="1">
         <v>46</v>
       </c>
-      <c r="E46" t="s">
-        <v>15</v>
-      </c>
-      <c r="F46" t="s">
+      <c r="E46" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="F46" s="1" t="s">
         <v>187</v>
       </c>
-      <c r="G46">
+      <c r="G46" s="1">
         <v>8397.92</v>
       </c>
     </row>
     <row r="47" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A47" t="s">
+      <c r="A47" s="1" t="s">
         <v>188</v>
       </c>
-      <c r="B47" t="s">
+      <c r="B47" s="1" t="s">
         <v>189</v>
       </c>
-      <c r="C47" t="s">
+      <c r="C47" s="1" t="s">
         <v>190</v>
       </c>
-      <c r="D47">
-        <v>15</v>
-      </c>
-      <c r="E47" t="s">
-        <v>10</v>
-      </c>
-      <c r="F47" t="s">
+      <c r="D47" s="1">
+        <v>15</v>
+      </c>
+      <c r="E47" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="F47" s="1" t="s">
         <v>191</v>
       </c>
-      <c r="G47">
+      <c r="G47" s="1">
         <v>1116.7</v>
       </c>
     </row>
     <row r="48" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A48" t="s">
+      <c r="A48" s="1" t="s">
         <v>192</v>
       </c>
-      <c r="B48" t="s">
+      <c r="B48" s="1" t="s">
         <v>193</v>
       </c>
-      <c r="C48" t="s">
+      <c r="C48" s="1" t="s">
         <v>194</v>
       </c>
-      <c r="D48">
+      <c r="D48" s="1">
         <v>29</v>
       </c>
-      <c r="E48" t="s">
-        <v>10</v>
-      </c>
-      <c r="F48" t="s">
+      <c r="E48" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="F48" s="1" t="s">
         <v>195</v>
       </c>
-      <c r="G48">
+      <c r="G48" s="1">
         <v>7803.64</v>
       </c>
     </row>
     <row r="49" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A49" t="s">
+      <c r="A49" s="1" t="s">
         <v>196</v>
       </c>
-      <c r="B49" t="s">
+      <c r="B49" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="C49" t="s">
+      <c r="C49" s="1" t="s">
         <v>197</v>
       </c>
-      <c r="D49">
+      <c r="D49" s="1">
         <v>23</v>
       </c>
-      <c r="E49" t="s">
-        <v>15</v>
-      </c>
-      <c r="F49" t="s">
+      <c r="E49" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="F49" s="1" t="s">
         <v>198</v>
       </c>
-      <c r="G49">
+      <c r="G49" s="1">
         <v>5980.76</v>
       </c>
     </row>
     <row r="50" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A50" t="s">
+      <c r="A50" s="1" t="s">
         <v>199</v>
       </c>
-      <c r="B50" t="s">
+      <c r="B50" s="1" t="s">
         <v>74</v>
       </c>
-      <c r="C50" t="s">
+      <c r="C50" s="1" t="s">
         <v>200</v>
       </c>
-      <c r="D50">
+      <c r="D50" s="1">
         <v>48</v>
       </c>
-      <c r="E50" t="s">
-        <v>10</v>
-      </c>
-      <c r="F50" t="s">
+      <c r="E50" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="F50" s="1" t="s">
         <v>201</v>
       </c>
-      <c r="G50">
+      <c r="G50" s="1">
         <v>9075.98</v>
       </c>
     </row>
     <row r="51" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A51" t="s">
+      <c r="A51" s="1" t="s">
         <v>202</v>
       </c>
-      <c r="B51" t="s">
+      <c r="B51" s="1" t="s">
         <v>203</v>
       </c>
-      <c r="C51" t="s">
+      <c r="C51" s="1" t="s">
         <v>204</v>
       </c>
-      <c r="D51">
+      <c r="D51" s="1">
         <v>41</v>
       </c>
-      <c r="E51" t="s">
-        <v>10</v>
-      </c>
-      <c r="F51" t="s">
+      <c r="E51" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="F51" s="1" t="s">
         <v>205</v>
       </c>
-      <c r="G51">
+      <c r="G51" s="1">
         <v>4068.87</v>
       </c>
     </row>
     <row r="52" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A52" t="s">
+      <c r="A52" s="1" t="s">
         <v>206</v>
       </c>
-      <c r="B52" t="s">
+      <c r="B52" s="1" t="s">
         <v>207</v>
       </c>
-      <c r="C52" t="s">
+      <c r="C52" s="1" t="s">
         <v>208</v>
       </c>
-      <c r="D52">
+      <c r="D52" s="1">
         <v>21</v>
       </c>
-      <c r="E52" t="s">
-        <v>15</v>
-      </c>
-      <c r="F52" t="s">
+      <c r="E52" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="F52" s="1" t="s">
         <v>209</v>
       </c>
-      <c r="G52">
+      <c r="G52" s="1">
         <v>1398.26</v>
       </c>
     </row>
     <row r="53" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A53" t="s">
+      <c r="A53" s="1" t="s">
         <v>210</v>
       </c>
-      <c r="B53" t="s">
+      <c r="B53" s="1" t="s">
         <v>211</v>
       </c>
-      <c r="C53" t="s">
+      <c r="C53" s="1" t="s">
         <v>212</v>
       </c>
-      <c r="D53">
+      <c r="D53" s="1">
         <v>43</v>
       </c>
-      <c r="E53" t="s">
-        <v>15</v>
-      </c>
-      <c r="F53" t="s">
+      <c r="E53" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="F53" s="1" t="s">
         <v>213</v>
       </c>
-      <c r="G53">
+      <c r="G53" s="1">
         <v>8895.57</v>
       </c>
     </row>
     <row r="54" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A54" t="s">
+      <c r="A54" s="1" t="s">
         <v>214</v>
       </c>
-      <c r="B54" t="s">
+      <c r="B54" s="1" t="s">
         <v>215</v>
       </c>
-      <c r="C54" t="s">
+      <c r="C54" s="1" t="s">
         <v>216</v>
       </c>
-      <c r="D54">
+      <c r="D54" s="1">
         <v>52</v>
       </c>
-      <c r="E54" t="s">
-        <v>15</v>
-      </c>
-      <c r="F54" t="s">
+      <c r="E54" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="F54" s="1" t="s">
         <v>217</v>
       </c>
-      <c r="G54">
+      <c r="G54" s="1">
         <v>6912.27</v>
       </c>
     </row>
     <row r="55" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A55" t="s">
+      <c r="A55" s="1" t="s">
         <v>218</v>
       </c>
-      <c r="B55" t="s">
+      <c r="B55" s="1" t="s">
         <v>219</v>
       </c>
-      <c r="C55" t="s">
+      <c r="C55" s="1" t="s">
         <v>220</v>
       </c>
-      <c r="D55">
+      <c r="D55" s="1">
         <v>33</v>
       </c>
-      <c r="E55" t="s">
-        <v>10</v>
-      </c>
-      <c r="F55" t="s">
+      <c r="E55" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="F55" s="1" t="s">
         <v>221</v>
       </c>
-      <c r="G55">
+      <c r="G55" s="1">
         <v>2324.0300000000002</v>
       </c>
     </row>
     <row r="56" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A56" t="s">
+      <c r="A56" s="1" t="s">
         <v>222</v>
       </c>
-      <c r="B56" t="s">
+      <c r="B56" s="1" t="s">
         <v>223</v>
       </c>
-      <c r="C56" t="s">
+      <c r="C56" s="1" t="s">
         <v>224</v>
       </c>
-      <c r="D56">
+      <c r="D56" s="1">
         <v>27</v>
       </c>
-      <c r="E56" t="s">
-        <v>15</v>
-      </c>
-      <c r="F56" t="s">
+      <c r="E56" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="F56" s="1" t="s">
         <v>225</v>
       </c>
-      <c r="G56">
+      <c r="G56" s="1">
         <v>535.38</v>
       </c>
     </row>
     <row r="57" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A57" t="s">
+      <c r="A57" s="1" t="s">
         <v>226</v>
       </c>
-      <c r="B57" t="s">
+      <c r="B57" s="1" t="s">
         <v>227</v>
       </c>
-      <c r="C57" t="s">
+      <c r="C57" s="1" t="s">
         <v>228</v>
       </c>
-      <c r="D57">
+      <c r="D57" s="1">
         <v>54</v>
       </c>
-      <c r="E57" t="s">
-        <v>15</v>
-      </c>
-      <c r="F57" t="s">
+      <c r="E57" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="F57" s="1" t="s">
         <v>229</v>
       </c>
-      <c r="G57">
+      <c r="G57" s="1">
         <v>8126.1</v>
       </c>
     </row>
     <row r="58" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A58" t="s">
+      <c r="A58" s="1" t="s">
         <v>230</v>
       </c>
-      <c r="B58" t="s">
+      <c r="B58" s="1" t="s">
         <v>231</v>
       </c>
-      <c r="C58" t="s">
+      <c r="C58" s="1" t="s">
         <v>232</v>
       </c>
-      <c r="D58">
+      <c r="D58" s="1">
         <v>39</v>
       </c>
-      <c r="E58" t="s">
-        <v>15</v>
-      </c>
-      <c r="F58" t="s">
+      <c r="E58" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="F58" s="1" t="s">
         <v>233</v>
       </c>
-      <c r="G58">
+      <c r="G58" s="1">
         <v>2169.54</v>
       </c>
     </row>
     <row r="59" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A59" t="s">
+      <c r="A59" s="1" t="s">
         <v>234</v>
       </c>
-      <c r="B59" t="s">
+      <c r="B59" s="1" t="s">
         <v>235</v>
       </c>
-      <c r="C59" t="s">
+      <c r="C59" s="1" t="s">
         <v>236</v>
       </c>
-      <c r="D59">
+      <c r="D59" s="1">
         <v>47</v>
       </c>
-      <c r="E59" t="s">
-        <v>10</v>
-      </c>
-      <c r="F59" t="s">
+      <c r="E59" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="F59" s="1" t="s">
         <v>237</v>
       </c>
-      <c r="G59">
+      <c r="G59" s="1">
         <v>7160.57</v>
       </c>
     </row>
     <row r="60" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A60" t="s">
+      <c r="A60" s="1" t="s">
         <v>238</v>
       </c>
-      <c r="B60" t="s">
+      <c r="B60" s="1" t="s">
         <v>239</v>
       </c>
-      <c r="C60" t="s">
+      <c r="C60" s="1" t="s">
         <v>240</v>
       </c>
-      <c r="D60">
+      <c r="D60" s="1">
         <v>60</v>
       </c>
-      <c r="E60" t="s">
-        <v>10</v>
-      </c>
-      <c r="F60" t="s">
+      <c r="E60" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="F60" s="1" t="s">
         <v>241</v>
       </c>
-      <c r="G60">
+      <c r="G60" s="1">
         <v>6829.48</v>
       </c>
     </row>
     <row r="61" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A61" t="s">
+      <c r="A61" s="1" t="s">
         <v>242</v>
       </c>
-      <c r="B61" t="s">
+      <c r="B61" s="1" t="s">
         <v>243</v>
       </c>
-      <c r="C61" t="s">
+      <c r="C61" s="1" t="s">
         <v>244</v>
       </c>
-      <c r="D61">
+      <c r="D61" s="1">
         <v>45</v>
       </c>
-      <c r="E61" t="s">
-        <v>15</v>
-      </c>
-      <c r="F61" t="s">
+      <c r="E61" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="F61" s="1" t="s">
         <v>245</v>
       </c>
-      <c r="G61">
+      <c r="G61" s="1">
         <v>2381.8000000000002</v>
       </c>
     </row>
     <row r="62" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A62" t="s">
+      <c r="A62" s="1" t="s">
         <v>246</v>
       </c>
-      <c r="B62" t="s">
+      <c r="B62" s="1" t="s">
         <v>247</v>
       </c>
-      <c r="C62" t="s">
+      <c r="C62" s="1" t="s">
         <v>248</v>
       </c>
-      <c r="D62">
+      <c r="D62" s="1">
         <v>21</v>
       </c>
-      <c r="E62" t="s">
-        <v>10</v>
-      </c>
-      <c r="F62" t="s">
+      <c r="E62" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="F62" s="1" t="s">
         <v>249</v>
       </c>
-      <c r="G62">
+      <c r="G62" s="1">
         <v>1750.13</v>
       </c>
     </row>
     <row r="63" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A63" t="s">
+      <c r="A63" s="1" t="s">
         <v>250</v>
       </c>
-      <c r="B63" t="s">
+      <c r="B63" s="1" t="s">
         <v>215</v>
       </c>
-      <c r="C63" t="s">
+      <c r="C63" s="1" t="s">
         <v>251</v>
       </c>
-      <c r="D63">
+      <c r="D63" s="1">
         <v>45</v>
       </c>
-      <c r="E63" t="s">
-        <v>10</v>
-      </c>
-      <c r="F63" t="s">
+      <c r="E63" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="F63" s="1" t="s">
         <v>252</v>
       </c>
-      <c r="G63">
+      <c r="G63" s="1">
         <v>7321.65</v>
       </c>
     </row>
     <row r="64" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A64" t="s">
+      <c r="A64" s="1" t="s">
         <v>253</v>
       </c>
-      <c r="B64" t="s">
+      <c r="B64" s="1" t="s">
         <v>254</v>
       </c>
-      <c r="C64" t="s">
+      <c r="C64" s="1" t="s">
         <v>255</v>
       </c>
-      <c r="D64">
+      <c r="D64" s="1">
         <v>26</v>
       </c>
-      <c r="E64" t="s">
-        <v>15</v>
-      </c>
-      <c r="F64" t="s">
+      <c r="E64" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="F64" s="1" t="s">
         <v>256</v>
       </c>
-      <c r="G64">
+      <c r="G64" s="1">
         <v>9369.5</v>
       </c>
     </row>
     <row r="65" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A65" t="s">
+      <c r="A65" s="1" t="s">
         <v>257</v>
       </c>
-      <c r="B65" t="s">
+      <c r="B65" s="1" t="s">
         <v>258</v>
       </c>
-      <c r="C65" t="s">
+      <c r="C65" s="1" t="s">
         <v>259</v>
       </c>
-      <c r="D65">
+      <c r="D65" s="1">
         <v>29</v>
       </c>
-      <c r="E65" t="s">
-        <v>15</v>
-      </c>
-      <c r="F65" t="s">
+      <c r="E65" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="F65" s="1" t="s">
         <v>260</v>
       </c>
-      <c r="G65">
+      <c r="G65" s="1">
         <v>8971.66</v>
       </c>
     </row>
     <row r="66" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A66" t="s">
+      <c r="A66" s="1" t="s">
         <v>261</v>
       </c>
-      <c r="B66" t="s">
+      <c r="B66" s="1" t="s">
         <v>262</v>
       </c>
-      <c r="C66" t="s">
+      <c r="C66" s="1" t="s">
         <v>263</v>
       </c>
-      <c r="D66">
+      <c r="D66" s="1">
         <v>49</v>
       </c>
-      <c r="E66" t="s">
-        <v>15</v>
-      </c>
-      <c r="F66" t="s">
+      <c r="E66" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="F66" s="1" t="s">
         <v>264</v>
       </c>
-      <c r="G66">
+      <c r="G66" s="1">
         <v>6788.09</v>
       </c>
     </row>
     <row r="67" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A67" t="s">
+      <c r="A67" s="1" t="s">
         <v>265</v>
       </c>
-      <c r="B67" t="s">
+      <c r="B67" s="1" t="s">
         <v>266</v>
       </c>
-      <c r="C67" t="s">
+      <c r="C67" s="1" t="s">
         <v>267</v>
       </c>
-      <c r="D67">
-        <v>15</v>
-      </c>
-      <c r="E67" t="s">
-        <v>10</v>
-      </c>
-      <c r="F67" t="s">
+      <c r="D67" s="1">
+        <v>15</v>
+      </c>
+      <c r="E67" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="F67" s="1" t="s">
         <v>268</v>
       </c>
-      <c r="G67">
+      <c r="G67" s="1">
         <v>8107.1</v>
       </c>
     </row>
     <row r="68" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A68" t="s">
+      <c r="A68" s="1" t="s">
         <v>269</v>
       </c>
-      <c r="B68" t="s">
+      <c r="B68" s="1" t="s">
         <v>270</v>
       </c>
-      <c r="C68" t="s">
+      <c r="C68" s="1" t="s">
         <v>271</v>
       </c>
-      <c r="D68">
+      <c r="D68" s="1">
         <v>18</v>
       </c>
-      <c r="E68" t="s">
-        <v>15</v>
-      </c>
-      <c r="F68" t="s">
+      <c r="E68" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="F68" s="1" t="s">
         <v>272</v>
       </c>
-      <c r="G68">
+      <c r="G68" s="1">
         <v>1929.31</v>
       </c>
     </row>
     <row r="69" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A69" t="s">
+      <c r="A69" s="1" t="s">
         <v>273</v>
       </c>
-      <c r="B69" t="s">
+      <c r="B69" s="1" t="s">
         <v>274</v>
       </c>
-      <c r="C69" t="s">
+      <c r="C69" s="1" t="s">
         <v>275</v>
       </c>
-      <c r="D69">
-        <v>15</v>
-      </c>
-      <c r="E69" t="s">
-        <v>15</v>
-      </c>
-      <c r="F69" t="s">
+      <c r="D69" s="1">
+        <v>15</v>
+      </c>
+      <c r="E69" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="F69" s="1" t="s">
         <v>276</v>
       </c>
-      <c r="G69">
+      <c r="G69" s="1">
         <v>8088.66</v>
       </c>
     </row>
     <row r="70" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A70" t="s">
+      <c r="A70" s="1" t="s">
         <v>277</v>
       </c>
-      <c r="B70" t="s">
+      <c r="B70" s="1" t="s">
         <v>278</v>
       </c>
-      <c r="C70" t="s">
+      <c r="C70" s="1" t="s">
         <v>279</v>
       </c>
-      <c r="D70">
+      <c r="D70" s="1">
         <v>42</v>
       </c>
-      <c r="E70" t="s">
-        <v>15</v>
-      </c>
-      <c r="F70" t="s">
+      <c r="E70" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="F70" s="1" t="s">
         <v>280</v>
       </c>
-      <c r="G70">
+      <c r="G70" s="1">
         <v>3860.38</v>
       </c>
     </row>
     <row r="71" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A71" t="s">
+      <c r="A71" s="1" t="s">
         <v>281</v>
       </c>
-      <c r="B71" t="s">
+      <c r="B71" s="1" t="s">
         <v>282</v>
       </c>
-      <c r="C71" t="s">
+      <c r="C71" s="1" t="s">
         <v>283</v>
       </c>
-      <c r="D71">
+      <c r="D71" s="1">
         <v>43</v>
       </c>
-      <c r="E71" t="s">
-        <v>10</v>
-      </c>
-      <c r="F71" t="s">
+      <c r="E71" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="F71" s="1" t="s">
         <v>284</v>
       </c>
-      <c r="G71">
+      <c r="G71" s="1">
         <v>5918.39</v>
       </c>
     </row>
     <row r="72" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A72" t="s">
+      <c r="A72" s="1" t="s">
         <v>285</v>
       </c>
-      <c r="B72" t="s">
+      <c r="B72" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="C72" t="s">
+      <c r="C72" s="1" t="s">
         <v>286</v>
       </c>
-      <c r="D72">
+      <c r="D72" s="1">
         <v>58</v>
       </c>
-      <c r="E72" t="s">
-        <v>15</v>
-      </c>
-      <c r="F72" t="s">
+      <c r="E72" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="F72" s="1" t="s">
         <v>287</v>
       </c>
-      <c r="G72">
+      <c r="G72" s="1">
         <v>4239.75</v>
       </c>
     </row>
     <row r="73" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A73" t="s">
+      <c r="A73" s="1" t="s">
         <v>288</v>
       </c>
-      <c r="B73" t="s">
+      <c r="B73" s="1" t="s">
         <v>289</v>
       </c>
-      <c r="C73" t="s">
+      <c r="C73" s="1" t="s">
         <v>290</v>
       </c>
-      <c r="D73">
+      <c r="D73" s="1">
         <v>25</v>
       </c>
-      <c r="E73" t="s">
-        <v>10</v>
-      </c>
-      <c r="F73" t="s">
+      <c r="E73" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="F73" s="1" t="s">
         <v>291</v>
       </c>
-      <c r="G73">
+      <c r="G73" s="1">
         <v>6392.62</v>
       </c>
     </row>
     <row r="74" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A74" t="s">
+      <c r="A74" s="1" t="s">
         <v>292</v>
       </c>
-      <c r="B74" t="s">
+      <c r="B74" s="1" t="s">
         <v>293</v>
       </c>
-      <c r="C74" t="s">
+      <c r="C74" s="1" t="s">
         <v>294</v>
       </c>
-      <c r="D74">
+      <c r="D74" s="1">
         <v>17</v>
       </c>
-      <c r="E74" t="s">
-        <v>10</v>
-      </c>
-      <c r="F74" t="s">
+      <c r="E74" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="F74" s="1" t="s">
         <v>295</v>
       </c>
-      <c r="G74">
+      <c r="G74" s="1">
         <v>8300.6200000000008</v>
       </c>
     </row>
     <row r="75" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A75" t="s">
+      <c r="A75" s="1" t="s">
         <v>296</v>
       </c>
-      <c r="B75" t="s">
+      <c r="B75" s="1" t="s">
         <v>297</v>
       </c>
-      <c r="C75" t="s">
+      <c r="C75" s="1" t="s">
         <v>298</v>
       </c>
-      <c r="D75">
-        <v>15</v>
-      </c>
-      <c r="E75" t="s">
-        <v>10</v>
-      </c>
-      <c r="F75" t="s">
+      <c r="D75" s="1">
+        <v>15</v>
+      </c>
+      <c r="E75" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="F75" s="1" t="s">
         <v>299</v>
       </c>
-      <c r="G75">
+      <c r="G75" s="1">
         <v>8059.69</v>
       </c>
     </row>
     <row r="76" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A76" t="s">
+      <c r="A76" s="1" t="s">
         <v>300</v>
       </c>
-      <c r="B76" t="s">
+      <c r="B76" s="1" t="s">
         <v>301</v>
       </c>
-      <c r="C76" t="s">
+      <c r="C76" s="1" t="s">
         <v>302</v>
       </c>
-      <c r="D76">
+      <c r="D76" s="1">
         <v>58</v>
       </c>
-      <c r="E76" t="s">
-        <v>10</v>
-      </c>
-      <c r="F76" t="s">
+      <c r="E76" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="F76" s="1" t="s">
         <v>303</v>
       </c>
-      <c r="G76">
+      <c r="G76" s="1">
         <v>1552.31</v>
       </c>
     </row>
     <row r="77" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A77" t="s">
+      <c r="A77" s="1" t="s">
         <v>304</v>
       </c>
-      <c r="B77" t="s">
+      <c r="B77" s="1" t="s">
         <v>305</v>
       </c>
-      <c r="C77" t="s">
+      <c r="C77" s="1" t="s">
         <v>306</v>
       </c>
-      <c r="D77">
+      <c r="D77" s="1">
         <v>37</v>
       </c>
-      <c r="E77" t="s">
-        <v>15</v>
-      </c>
-      <c r="F77" t="s">
+      <c r="E77" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="F77" s="1" t="s">
         <v>307</v>
       </c>
-      <c r="G77">
+      <c r="G77" s="1">
         <v>5437.66</v>
       </c>
     </row>
     <row r="78" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A78" t="s">
+      <c r="A78" s="1" t="s">
         <v>308</v>
       </c>
-      <c r="B78" t="s">
+      <c r="B78" s="1" t="s">
         <v>309</v>
       </c>
-      <c r="C78" t="s">
+      <c r="C78" s="1" t="s">
         <v>310</v>
       </c>
-      <c r="D78">
+      <c r="D78" s="1">
         <v>32</v>
       </c>
-      <c r="E78" t="s">
-        <v>15</v>
-      </c>
-      <c r="F78" t="s">
+      <c r="E78" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="F78" s="1" t="s">
         <v>311</v>
       </c>
-      <c r="G78">
+      <c r="G78" s="1">
         <v>4166.07</v>
       </c>
     </row>
     <row r="79" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A79" t="s">
+      <c r="A79" s="1" t="s">
         <v>312</v>
       </c>
-      <c r="B79" t="s">
+      <c r="B79" s="1" t="s">
         <v>313</v>
       </c>
-      <c r="C79" t="s">
+      <c r="C79" s="1" t="s">
         <v>314</v>
       </c>
-      <c r="D79">
+      <c r="D79" s="1">
         <v>34</v>
       </c>
-      <c r="E79" t="s">
-        <v>15</v>
-      </c>
-      <c r="F79" t="s">
+      <c r="E79" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="F79" s="1" t="s">
         <v>315</v>
       </c>
-      <c r="G79">
+      <c r="G79" s="1">
         <v>666.78</v>
       </c>
     </row>
     <row r="80" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A80" t="s">
+      <c r="A80" s="1" t="s">
         <v>316</v>
       </c>
-      <c r="B80" t="s">
+      <c r="B80" s="1" t="s">
         <v>317</v>
       </c>
-      <c r="C80" t="s">
+      <c r="C80" s="1" t="s">
         <v>318</v>
       </c>
-      <c r="D80">
+      <c r="D80" s="1">
         <v>51</v>
       </c>
-      <c r="E80" t="s">
-        <v>15</v>
-      </c>
-      <c r="F80" t="s">
+      <c r="E80" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="F80" s="1" t="s">
         <v>319</v>
       </c>
-      <c r="G80">
+      <c r="G80" s="1">
         <v>7911.6</v>
       </c>
     </row>
     <row r="81" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A81" t="s">
+      <c r="A81" s="1" t="s">
         <v>320</v>
       </c>
-      <c r="B81" t="s">
+      <c r="B81" s="1" t="s">
         <v>321</v>
       </c>
-      <c r="C81" t="s">
+      <c r="C81" s="1" t="s">
         <v>322</v>
       </c>
-      <c r="D81">
+      <c r="D81" s="1">
         <v>26</v>
       </c>
-      <c r="E81" t="s">
-        <v>10</v>
-      </c>
-      <c r="F81" t="s">
+      <c r="E81" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="F81" s="1" t="s">
         <v>323</v>
       </c>
-      <c r="G81">
+      <c r="G81" s="1">
         <v>7375.74</v>
       </c>
     </row>
     <row r="82" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A82" t="s">
+      <c r="A82" s="1" t="s">
         <v>324</v>
       </c>
-      <c r="B82" t="s">
+      <c r="B82" s="1" t="s">
         <v>110</v>
       </c>
-      <c r="C82" t="s">
+      <c r="C82" s="1" t="s">
         <v>228</v>
       </c>
-      <c r="D82">
+      <c r="D82" s="1">
         <v>56</v>
       </c>
-      <c r="E82" t="s">
-        <v>10</v>
-      </c>
-      <c r="F82" t="s">
+      <c r="E82" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="F82" s="1" t="s">
         <v>325</v>
       </c>
-      <c r="G82">
+      <c r="G82" s="1">
         <v>3272.37</v>
       </c>
     </row>
     <row r="83" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A83" t="s">
+      <c r="A83" s="1" t="s">
         <v>326</v>
       </c>
-      <c r="B83" t="s">
+      <c r="B83" s="1" t="s">
         <v>327</v>
       </c>
-      <c r="C83" t="s">
+      <c r="C83" s="1" t="s">
         <v>328</v>
       </c>
-      <c r="D83">
+      <c r="D83" s="1">
         <v>40</v>
       </c>
-      <c r="E83" t="s">
-        <v>10</v>
-      </c>
-      <c r="F83" t="s">
+      <c r="E83" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="F83" s="1" t="s">
         <v>329</v>
       </c>
-      <c r="G83">
+      <c r="G83" s="1">
         <v>485.05</v>
       </c>
     </row>
     <row r="84" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A84" t="s">
+      <c r="A84" s="1" t="s">
         <v>330</v>
       </c>
-      <c r="B84" t="s">
+      <c r="B84" s="1" t="s">
         <v>331</v>
       </c>
-      <c r="C84" t="s">
+      <c r="C84" s="1" t="s">
         <v>332</v>
       </c>
-      <c r="D84">
+      <c r="D84" s="1">
         <v>38</v>
       </c>
-      <c r="E84" t="s">
-        <v>15</v>
-      </c>
-      <c r="F84" t="s">
+      <c r="E84" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="F84" s="1" t="s">
         <v>333</v>
       </c>
-      <c r="G84">
+      <c r="G84" s="1">
         <v>1114.8599999999999</v>
       </c>
     </row>
     <row r="85" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A85" t="s">
+      <c r="A85" s="1" t="s">
         <v>334</v>
       </c>
-      <c r="B85" t="s">
+      <c r="B85" s="1" t="s">
         <v>335</v>
       </c>
-      <c r="C85" t="s">
+      <c r="C85" s="1" t="s">
         <v>336</v>
       </c>
-      <c r="D85">
+      <c r="D85" s="1">
         <v>54</v>
       </c>
-      <c r="E85" t="s">
-        <v>10</v>
-      </c>
-      <c r="F85" t="s">
+      <c r="E85" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="F85" s="1" t="s">
         <v>337</v>
       </c>
-      <c r="G85">
+      <c r="G85" s="1">
         <v>1144.24</v>
       </c>
     </row>
     <row r="86" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A86" t="s">
+      <c r="A86" s="1" t="s">
         <v>338</v>
       </c>
-      <c r="B86" t="s">
+      <c r="B86" s="1" t="s">
         <v>339</v>
       </c>
-      <c r="C86" t="s">
+      <c r="C86" s="1" t="s">
         <v>340</v>
       </c>
-      <c r="D86">
+      <c r="D86" s="1">
         <v>17</v>
       </c>
-      <c r="E86" t="s">
-        <v>10</v>
-      </c>
-      <c r="F86" t="s">
+      <c r="E86" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="F86" s="1" t="s">
         <v>341</v>
       </c>
-      <c r="G86">
+      <c r="G86" s="1">
         <v>3334.11</v>
       </c>
     </row>
     <row r="87" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A87" t="s">
+      <c r="A87" s="1" t="s">
         <v>342</v>
       </c>
-      <c r="B87" t="s">
+      <c r="B87" s="1" t="s">
         <v>343</v>
       </c>
-      <c r="C87" t="s">
+      <c r="C87" s="1" t="s">
         <v>344</v>
       </c>
-      <c r="D87">
+      <c r="D87" s="1">
         <v>34</v>
       </c>
-      <c r="E87" t="s">
-        <v>15</v>
-      </c>
-      <c r="F87" t="s">
+      <c r="E87" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="F87" s="1" t="s">
         <v>345</v>
       </c>
-      <c r="G87">
+      <c r="G87" s="1">
         <v>8829.91</v>
       </c>
     </row>
     <row r="88" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A88" t="s">
+      <c r="A88" s="1" t="s">
         <v>346</v>
       </c>
-      <c r="B88" t="s">
+      <c r="B88" s="1" t="s">
         <v>347</v>
       </c>
-      <c r="C88" t="s">
+      <c r="C88" s="1" t="s">
         <v>348</v>
       </c>
-      <c r="D88">
+      <c r="D88" s="1">
         <v>38</v>
       </c>
-      <c r="E88" t="s">
-        <v>15</v>
-      </c>
-      <c r="F88" t="s">
+      <c r="E88" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="F88" s="1" t="s">
         <v>349</v>
       </c>
-      <c r="G88">
+      <c r="G88" s="1">
         <v>5634.03</v>
       </c>
     </row>
     <row r="89" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A89" t="s">
+      <c r="A89" s="1" t="s">
         <v>350</v>
       </c>
-      <c r="B89" t="s">
+      <c r="B89" s="1" t="s">
         <v>351</v>
       </c>
-      <c r="C89" t="s">
+      <c r="C89" s="1" t="s">
         <v>224</v>
       </c>
-      <c r="D89">
+      <c r="D89" s="1">
         <v>44</v>
       </c>
-      <c r="E89" t="s">
-        <v>10</v>
-      </c>
-      <c r="F89" t="s">
+      <c r="E89" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="F89" s="1" t="s">
         <v>352</v>
       </c>
-      <c r="G89">
+      <c r="G89" s="1">
         <v>4408.8999999999996</v>
       </c>
     </row>
     <row r="90" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A90" t="s">
+      <c r="A90" s="1" t="s">
         <v>353</v>
       </c>
-      <c r="B90" t="s">
+      <c r="B90" s="1" t="s">
         <v>354</v>
       </c>
-      <c r="C90" t="s">
+      <c r="C90" s="1" t="s">
         <v>355</v>
       </c>
-      <c r="D90">
+      <c r="D90" s="1">
         <v>30</v>
       </c>
-      <c r="E90" t="s">
-        <v>10</v>
-      </c>
-      <c r="F90" t="s">
+      <c r="E90" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="F90" s="1" t="s">
         <v>356</v>
       </c>
-      <c r="G90">
+      <c r="G90" s="1">
         <v>2283.4699999999998</v>
       </c>
     </row>
     <row r="91" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A91" t="s">
+      <c r="A91" s="1" t="s">
         <v>357</v>
       </c>
-      <c r="B91" t="s">
+      <c r="B91" s="1" t="s">
         <v>358</v>
       </c>
-      <c r="C91" t="s">
+      <c r="C91" s="1" t="s">
         <v>359</v>
       </c>
-      <c r="D91">
+      <c r="D91" s="1">
         <v>56</v>
       </c>
-      <c r="E91" t="s">
-        <v>15</v>
-      </c>
-      <c r="F91" t="s">
+      <c r="E91" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="F91" s="1" t="s">
         <v>360</v>
       </c>
-      <c r="G91">
+      <c r="G91" s="1">
         <v>695.29</v>
       </c>
     </row>
     <row r="92" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A92" t="s">
+      <c r="A92" s="1" t="s">
         <v>361</v>
       </c>
-      <c r="B92" t="s">
+      <c r="B92" s="1" t="s">
         <v>362</v>
       </c>
-      <c r="C92" t="s">
+      <c r="C92" s="1" t="s">
         <v>363</v>
       </c>
-      <c r="D92">
+      <c r="D92" s="1">
         <v>41</v>
       </c>
-      <c r="E92" t="s">
-        <v>15</v>
-      </c>
-      <c r="F92" t="s">
+      <c r="E92" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="F92" s="1" t="s">
         <v>364</v>
       </c>
-      <c r="G92">
+      <c r="G92" s="1">
         <v>4649.95</v>
       </c>
     </row>
     <row r="93" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A93" t="s">
+      <c r="A93" s="1" t="s">
         <v>365</v>
       </c>
-      <c r="B93" t="s">
+      <c r="B93" s="1" t="s">
         <v>366</v>
       </c>
-      <c r="C93" t="s">
+      <c r="C93" s="1" t="s">
         <v>367</v>
       </c>
-      <c r="D93">
+      <c r="D93" s="1">
         <v>46</v>
       </c>
-      <c r="E93" t="s">
-        <v>10</v>
-      </c>
-      <c r="F93" t="s">
+      <c r="E93" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="F93" s="1" t="s">
         <v>368</v>
       </c>
-      <c r="G93">
+      <c r="G93" s="1">
         <v>946.11</v>
       </c>
     </row>
     <row r="94" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A94" t="s">
+      <c r="A94" s="1" t="s">
         <v>369</v>
       </c>
-      <c r="B94" t="s">
+      <c r="B94" s="1" t="s">
         <v>370</v>
       </c>
-      <c r="C94" t="s">
+      <c r="C94" s="1" t="s">
         <v>371</v>
       </c>
-      <c r="D94">
+      <c r="D94" s="1">
         <v>34</v>
       </c>
-      <c r="E94" t="s">
-        <v>15</v>
-      </c>
-      <c r="F94" t="s">
+      <c r="E94" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="F94" s="1" t="s">
         <v>372</v>
       </c>
-      <c r="G94">
+      <c r="G94" s="1">
         <v>125.33</v>
       </c>
     </row>
     <row r="95" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A95" t="s">
+      <c r="A95" s="1" t="s">
         <v>373</v>
       </c>
-      <c r="B95" t="s">
+      <c r="B95" s="1" t="s">
         <v>374</v>
       </c>
-      <c r="C95" t="s">
+      <c r="C95" s="1" t="s">
         <v>375</v>
       </c>
-      <c r="D95">
+      <c r="D95" s="1">
         <v>35</v>
       </c>
-      <c r="E95" t="s">
-        <v>10</v>
-      </c>
-      <c r="F95" t="s">
+      <c r="E95" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="F95" s="1" t="s">
         <v>376</v>
       </c>
-      <c r="G95">
+      <c r="G95" s="1">
         <v>5811.17</v>
       </c>
     </row>
     <row r="96" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A96" t="s">
+      <c r="A96" s="1" t="s">
         <v>377</v>
       </c>
-      <c r="B96" t="s">
+      <c r="B96" s="1" t="s">
         <v>378</v>
       </c>
-      <c r="C96" t="s">
+      <c r="C96" s="1" t="s">
         <v>379</v>
       </c>
-      <c r="D96">
+      <c r="D96" s="1">
         <v>20</v>
       </c>
-      <c r="E96" t="s">
-        <v>10</v>
-      </c>
-      <c r="F96" t="s">
+      <c r="E96" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="F96" s="1" t="s">
         <v>380</v>
       </c>
-      <c r="G96">
+      <c r="G96" s="1">
         <v>7626.66</v>
       </c>
     </row>
     <row r="97" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A97" t="s">
+      <c r="A97" s="1" t="s">
         <v>381</v>
       </c>
-      <c r="B97" t="s">
+      <c r="B97" s="1" t="s">
         <v>382</v>
       </c>
-      <c r="C97" t="s">
+      <c r="C97" s="1" t="s">
         <v>383</v>
       </c>
-      <c r="D97">
+      <c r="D97" s="1">
         <v>19</v>
       </c>
-      <c r="E97" t="s">
-        <v>10</v>
-      </c>
-      <c r="F97" t="s">
+      <c r="E97" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="F97" s="1" t="s">
         <v>384</v>
       </c>
-      <c r="G97">
+      <c r="G97" s="1">
         <v>899.61</v>
       </c>
     </row>
     <row r="98" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A98" t="s">
+      <c r="A98" s="1" t="s">
         <v>385</v>
       </c>
-      <c r="B98" t="s">
+      <c r="B98" s="1" t="s">
         <v>386</v>
       </c>
-      <c r="C98" t="s">
+      <c r="C98" s="1" t="s">
         <v>387</v>
       </c>
-      <c r="D98">
+      <c r="D98" s="1">
         <v>31</v>
       </c>
-      <c r="E98" t="s">
-        <v>15</v>
-      </c>
-      <c r="F98" t="s">
+      <c r="E98" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="F98" s="1" t="s">
         <v>388</v>
       </c>
-      <c r="G98">
+      <c r="G98" s="1">
         <v>7563.52</v>
       </c>
     </row>
     <row r="99" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A99" t="s">
+      <c r="A99" s="1" t="s">
         <v>389</v>
       </c>
-      <c r="B99" t="s">
+      <c r="B99" s="1" t="s">
         <v>390</v>
       </c>
-      <c r="C99" t="s">
+      <c r="C99" s="1" t="s">
         <v>391</v>
       </c>
-      <c r="D99">
+      <c r="D99" s="1">
         <v>35</v>
       </c>
-      <c r="E99" t="s">
-        <v>10</v>
-      </c>
-      <c r="F99" t="s">
+      <c r="E99" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="F99" s="1" t="s">
         <v>392</v>
       </c>
-      <c r="G99">
+      <c r="G99" s="1">
         <v>7527.3</v>
       </c>
     </row>
     <row r="100" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A100" t="s">
+      <c r="A100" s="1" t="s">
         <v>393</v>
       </c>
-      <c r="B100" t="s">
+      <c r="B100" s="1" t="s">
         <v>394</v>
       </c>
-      <c r="C100" t="s">
+      <c r="C100" s="1" t="s">
         <v>395</v>
       </c>
-      <c r="D100">
+      <c r="D100" s="1">
         <v>29</v>
       </c>
-      <c r="E100" t="s">
-        <v>15</v>
-      </c>
-      <c r="F100" t="s">
+      <c r="E100" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="F100" s="1" t="s">
         <v>396</v>
       </c>
-      <c r="G100">
+      <c r="G100" s="1">
         <v>5061.12</v>
       </c>
     </row>
     <row r="101" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A101" t="s">
+      <c r="A101" s="1" t="s">
         <v>397</v>
       </c>
-      <c r="B101" t="s">
+      <c r="B101" s="1" t="s">
         <v>398</v>
       </c>
-      <c r="C101" t="s">
+      <c r="C101" s="1" t="s">
         <v>399</v>
       </c>
-      <c r="D101">
+      <c r="D101" s="1">
         <v>45</v>
       </c>
-      <c r="E101" t="s">
-        <v>10</v>
-      </c>
-      <c r="F101" t="s">
+      <c r="E101" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="F101" s="1" t="s">
         <v>400</v>
       </c>
-      <c r="G101">
+      <c r="G101" s="1">
         <v>2893.68</v>
       </c>
     </row>
   </sheetData>
   <sheetProtection formatCells="0" formatColumns="0" formatRows="0" insertColumns="0" insertRows="0" insertHyperlinks="0" deleteColumns="0" deleteRows="0" sort="0" autoFilter="0" pivotTables="0"/>
+  <hyperlinks>
+    <hyperlink ref="F2" r:id="rId1" xr:uid="{E0D70B53-1214-4ACE-AFE4-D62244EFC583}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Optimize bool and datetime auto check
</commit_message>
<xml_diff>
--- a/samples/xlsx/TestTypeMapping.xlsx
+++ b/samples/xlsx/TestTypeMapping.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\git\MiniExcel\samples\xlsx\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7725CD23-B626-49D6-88CC-412E88C9EB67}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4C5F89F2-95EA-46C1-AEF5-49D677682ACC}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-21720" yWindow="-120" windowWidth="21840" windowHeight="13290" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Worksheet" sheetId="1" r:id="rId1"/>
@@ -1585,7 +1585,7 @@
   <dimension ref="A1:H101"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J2" sqref="J2"/>
+      <selection activeCell="J10" sqref="J10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>